<commit_message>
values extracted from switch statement
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="B5:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,11 +421,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Origin CMM output</t>
-        </is>
+    <row r="5">
+      <c r="B5" t="n">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="D7" t="n">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="F10" t="n">
+        <v>2063</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extraxt values from report
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -423,17 +423,17 @@
   <sheetData>
     <row r="5">
       <c r="B5" t="n">
-        <v>3609</v>
+        <v>2918</v>
       </c>
     </row>
     <row r="7">
       <c r="D7" t="n">
-        <v>3693</v>
+        <v>3028</v>
       </c>
     </row>
     <row r="10">
       <c r="F10" t="n">
-        <v>2063</v>
+        <v>6418756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
copy a template and the format the output
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,16 +25,29 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -42,12 +55,80 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +494,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B5:F10"/>
+  <dimension ref="A1:AN100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,21 +502,155 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>CMM Report</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n"/>
+      <c r="C1" s="2" t="n"/>
+      <c r="D1" s="2" t="n"/>
+      <c r="E1" s="2" t="n"/>
+      <c r="F1" s="2" t="n"/>
+      <c r="G1" s="2" t="n"/>
+      <c r="H1" s="2" t="n"/>
+      <c r="I1" s="2" t="n"/>
+      <c r="J1" s="2" t="n"/>
+      <c r="K1" s="2" t="n"/>
+      <c r="L1" s="3" t="n"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n"/>
+      <c r="B2" s="5" t="n"/>
+      <c r="C2" s="5" t="n"/>
+      <c r="D2" s="5" t="n"/>
+      <c r="E2" s="5" t="n"/>
+      <c r="F2" s="5" t="n"/>
+      <c r="G2" s="5" t="n"/>
+      <c r="H2" s="5" t="n"/>
+      <c r="I2" s="5" t="n"/>
+      <c r="J2" s="5" t="n"/>
+      <c r="K2" s="5" t="n"/>
+      <c r="L2" s="6" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>this is a report from origin</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
     <row r="5">
       <c r="B5" t="n">
-        <v>2918</v>
+        <v>942</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1752</v>
+      </c>
+      <c r="D5" t="n">
+        <v>6418756</v>
+      </c>
+      <c r="E5" t="n">
+        <v>16</v>
       </c>
     </row>
-    <row r="7">
-      <c r="D7" t="n">
-        <v>3028</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="F10" t="n">
-        <v>6418756</v>
-      </c>
-    </row>
+    <row r="6"/>
+    <row r="7"/>
+    <row r="8"/>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
+    <row r="13"/>
+    <row r="14"/>
+    <row r="15"/>
+    <row r="16"/>
+    <row r="17"/>
+    <row r="18"/>
+    <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
+    <row r="26"/>
+    <row r="27"/>
+    <row r="28"/>
+    <row r="29"/>
+    <row r="30"/>
+    <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
+    <row r="53"/>
+    <row r="54"/>
+    <row r="55"/>
+    <row r="56"/>
+    <row r="57"/>
+    <row r="58"/>
+    <row r="59"/>
+    <row r="60"/>
+    <row r="61"/>
+    <row r="62"/>
+    <row r="63"/>
+    <row r="64"/>
+    <row r="65"/>
+    <row r="66"/>
+    <row r="67"/>
+    <row r="68"/>
+    <row r="69"/>
+    <row r="70"/>
+    <row r="71"/>
+    <row r="72"/>
+    <row r="73"/>
+    <row r="74"/>
+    <row r="75"/>
+    <row r="76"/>
+    <row r="77"/>
+    <row r="78"/>
+    <row r="79"/>
+    <row r="80"/>
+    <row r="81"/>
+    <row r="82"/>
+    <row r="83"/>
+    <row r="84"/>
+    <row r="85"/>
+    <row r="86"/>
+    <row r="87"/>
+    <row r="88"/>
+    <row r="89"/>
+    <row r="90"/>
+    <row r="91"/>
+    <row r="92"/>
+    <row r="93"/>
+    <row r="94"/>
+    <row r="95"/>
+    <row r="96"/>
+    <row r="97"/>
+    <row r="98"/>
+    <row r="99"/>
+    <row r="100"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
added cell spacing as well to make sure text is disaplayed over the all cell|
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="8">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,13 +27,57 @@
     </font>
     <font>
       <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="14"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="4"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <color theme="0"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -46,8 +90,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -55,80 +123,39 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -501,75 +528,284 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="23.6640625" customWidth="1" min="1" max="1"/>
+    <col width="18.33203125" customWidth="1" min="2" max="2"/>
+    <col width="25.33203125" customWidth="1" min="3" max="3"/>
+    <col width="22.6640625" customWidth="1" min="4" max="4"/>
+    <col width="22.33203125" customWidth="1" min="5" max="5"/>
+    <col width="25.1640625" customWidth="1" min="6" max="6"/>
+    <col width="17.33203125" customWidth="1" min="7" max="7"/>
+    <col width="13" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="13" customWidth="1" min="10" max="10"/>
+    <col width="13" customWidth="1" min="11" max="11"/>
+    <col width="13" customWidth="1" min="12" max="12"/>
+    <col width="13" customWidth="1" min="13" max="13"/>
+    <col width="13" customWidth="1" min="14" max="14"/>
+    <col width="13" customWidth="1" min="15" max="15"/>
+    <col width="13" customWidth="1" min="16" max="16"/>
+    <col width="13" customWidth="1" min="17" max="17"/>
+    <col width="13" customWidth="1" min="18" max="18"/>
+    <col width="13" customWidth="1" min="19" max="19"/>
+    <col width="13" customWidth="1" min="20" max="20"/>
+    <col width="13" customWidth="1" min="21" max="21"/>
+    <col width="13" customWidth="1" min="22" max="22"/>
+    <col width="13" customWidth="1" min="23" max="23"/>
+    <col width="13" customWidth="1" min="24" max="24"/>
+    <col width="13" customWidth="1" min="25" max="25"/>
+    <col width="13" customWidth="1" min="26" max="26"/>
+    <col width="13" customWidth="1" min="27" max="27"/>
+    <col width="13" customWidth="1" min="28" max="28"/>
+    <col width="13" customWidth="1" min="29" max="29"/>
+    <col width="13" customWidth="1" min="30" max="30"/>
+    <col width="13" customWidth="1" min="31" max="31"/>
+    <col width="13" customWidth="1" min="32" max="32"/>
+    <col width="13" customWidth="1" min="33" max="33"/>
+    <col width="13" customWidth="1" min="34" max="34"/>
+    <col width="13" customWidth="1" min="35" max="35"/>
+    <col width="13" customWidth="1" min="36" max="36"/>
+    <col width="13" customWidth="1" min="37" max="37"/>
+    <col width="13" customWidth="1" min="38" max="38"/>
+    <col width="13" customWidth="1" min="39" max="39"/>
+    <col width="13" customWidth="1" min="40" max="40"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="19" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CMM Report</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n"/>
-      <c r="C1" s="2" t="n"/>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
-      <c r="F1" s="2" t="n"/>
-      <c r="G1" s="2" t="n"/>
-      <c r="H1" s="2" t="n"/>
-      <c r="I1" s="2" t="n"/>
-      <c r="J1" s="2" t="n"/>
-      <c r="K1" s="2" t="n"/>
-      <c r="L1" s="3" t="n"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="n"/>
-      <c r="B2" s="5" t="n"/>
-      <c r="C2" s="5" t="n"/>
-      <c r="D2" s="5" t="n"/>
-      <c r="E2" s="5" t="n"/>
-      <c r="F2" s="5" t="n"/>
-      <c r="G2" s="5" t="n"/>
-      <c r="H2" s="5" t="n"/>
-      <c r="I2" s="5" t="n"/>
-      <c r="J2" s="5" t="n"/>
-      <c r="K2" s="5" t="n"/>
-      <c r="L2" s="6" t="n"/>
-    </row>
+          <t>Net Campaign Delivery - Reach and Frequency</t>
+        </is>
+      </c>
+    </row>
+    <row r="2"/>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>this is a report from origin</t>
-        </is>
-      </c>
-    </row>
-    <row r="4"/>
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Meaused Entity</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Media Type</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>Impression Filter</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>Impression Filter</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>total Campaign Reach</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>Total Net Campaign Reach %</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>Average Frequency</t>
+        </is>
+      </c>
+      <c r="H3" s="3" t="n"/>
+      <c r="I3" s="3" t="n"/>
+      <c r="J3" s="3" t="n"/>
+      <c r="K3" s="3" t="n"/>
+      <c r="L3" s="3" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Linear TV, Google</t>
+        </is>
+      </c>
+      <c r="B4" s="4" t="inlineStr">
+        <is>
+          <t>Video</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="inlineStr">
+        <is>
+          <t>MRC Standard</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
+          <t>MRC Standard</t>
+        </is>
+      </c>
+      <c r="E4" s="6" t="n">
+        <v>3944</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <v>2100</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>6418756</v>
+      </c>
+      <c r="H4" s="3" t="n"/>
+      <c r="I4" s="3" t="n"/>
+      <c r="J4" s="3" t="n"/>
+      <c r="K4" s="3" t="n"/>
+      <c r="L4" s="3" t="n"/>
+    </row>
     <row r="5">
-      <c r="B5" t="n">
-        <v>942</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1752</v>
-      </c>
-      <c r="D5" t="n">
-        <v>6418756</v>
-      </c>
-      <c r="E5" t="n">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Liner TV, Meta, Google</t>
+        </is>
+      </c>
+      <c r="B5" s="4" t="inlineStr">
+        <is>
+          <t>other, video</t>
+        </is>
+      </c>
+      <c r="C5" s="4" t="inlineStr">
+        <is>
+          <t>All Measurable Impressions</t>
+        </is>
+      </c>
+      <c r="D5" s="5" t="inlineStr">
+        <is>
+          <t>All Measurable Impressions</t>
+        </is>
+      </c>
+      <c r="E5" s="6" t="n">
         <v>16</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <v>16</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>1194</v>
       </c>
     </row>
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>
-    <row r="9"/>
+    <row r="9" ht="24" customHeight="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>Campaign duplication, unique reach and cross-over / overlap</t>
+        </is>
+      </c>
+      <c r="B9" s="8" t="n"/>
+    </row>
     <row r="10"/>
     <row r="11"/>
-    <row r="12"/>
-    <row r="13"/>
-    <row r="14"/>
-    <row r="15"/>
-    <row r="16"/>
-    <row r="17"/>
-    <row r="18"/>
-    <row r="19"/>
+    <row r="12">
+      <c r="A12" s="9" t="n"/>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>(Siloed) Gross Reach</t>
+        </is>
+      </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>Unique Reach</t>
+        </is>
+      </c>
+      <c r="E12" s="10" t="n"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="11" t="inlineStr">
+        <is>
+          <t>You Tube AMI</t>
+        </is>
+      </c>
+      <c r="B13" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_7}</t>
+        </is>
+      </c>
+      <c r="C13" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_11}</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="11" t="inlineStr">
+        <is>
+          <t>Liner TV AMI</t>
+        </is>
+      </c>
+      <c r="B14" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_8}</t>
+        </is>
+      </c>
+      <c r="C14" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_12}</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="11" t="inlineStr">
+        <is>
+          <t>Meta AMI</t>
+        </is>
+      </c>
+      <c r="B15" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_9}</t>
+        </is>
+      </c>
+      <c r="C15" s="12" t="inlineStr">
+        <is>
+          <t>{o_t_13}</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="13" t="inlineStr">
+        <is>
+          <t>total</t>
+        </is>
+      </c>
+      <c r="B16" s="14" t="inlineStr">
+        <is>
+          <t>{o_t_10}</t>
+        </is>
+      </c>
+      <c r="C16" s="14" t="inlineStr">
+        <is>
+          <t>{o_t_14}</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="34" customHeight="1">
+      <c r="A17" s="15" t="inlineStr">
+        <is>
+          <t>total duplicated Net Campaign Reach</t>
+        </is>
+      </c>
+      <c r="B17" s="16" t="inlineStr">
+        <is>
+          <t>33, 714, 428</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="17" t="n"/>
+      <c r="B18" s="17" t="n"/>
+    </row>
+    <row r="19">
+      <c r="H19" t="inlineStr">
+        <is>
+          <t> </t>
+        </is>
+      </c>
+    </row>
     <row r="20"/>
     <row r="21"/>
     <row r="22"/>

</xml_diff>

<commit_message>
extracting values from JSON
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -16,7 +16,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+  </numFmts>
   <fonts count="8">
     <font>
       <name val="Calibri"/>
@@ -127,13 +129,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -643,13 +648,13 @@
         </is>
       </c>
       <c r="E4" s="6" t="n">
-        <v>3944</v>
-      </c>
-      <c r="F4" s="6" t="n">
-        <v>2100</v>
-      </c>
-      <c r="G4" s="6" t="n">
-        <v>6418756</v>
+        <v>27714428</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>50.34</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>4.14</v>
       </c>
       <c r="H4" s="3" t="n"/>
       <c r="I4" s="3" t="n"/>
@@ -679,125 +684,125 @@
         </is>
       </c>
       <c r="E5" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="F5" s="6" t="n">
-        <v>16</v>
-      </c>
-      <c r="G5" s="6" t="n">
-        <v>1194</v>
+        <v>33714428</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>33714428</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>1203</v>
       </c>
     </row>
     <row r="6"/>
     <row r="7"/>
     <row r="8"/>
     <row r="9" ht="24" customHeight="1">
-      <c r="A9" s="7" t="inlineStr">
+      <c r="A9" s="8" t="inlineStr">
         <is>
           <t>Campaign duplication, unique reach and cross-over / overlap</t>
         </is>
       </c>
-      <c r="B9" s="8" t="n"/>
+      <c r="B9" s="9" t="n"/>
     </row>
     <row r="10"/>
     <row r="11"/>
     <row r="12">
-      <c r="A12" s="9" t="n"/>
-      <c r="B12" s="9" t="inlineStr">
+      <c r="A12" s="10" t="n"/>
+      <c r="B12" s="10" t="inlineStr">
         <is>
           <t>(Siloed) Gross Reach</t>
         </is>
       </c>
-      <c r="C12" s="9" t="inlineStr">
+      <c r="C12" s="10" t="inlineStr">
         <is>
           <t>Unique Reach</t>
         </is>
       </c>
-      <c r="E12" s="10" t="n"/>
+      <c r="E12" s="11" t="n"/>
     </row>
     <row r="13">
-      <c r="A13" s="11" t="inlineStr">
+      <c r="A13" s="12" t="inlineStr">
         <is>
           <t>You Tube AMI</t>
         </is>
       </c>
-      <c r="B13" s="12" t="inlineStr">
+      <c r="B13" s="13" t="inlineStr">
         <is>
           <t>{o_t_7}</t>
         </is>
       </c>
-      <c r="C13" s="12" t="inlineStr">
+      <c r="C13" s="13" t="inlineStr">
         <is>
           <t>{o_t_11}</t>
         </is>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="11" t="inlineStr">
+      <c r="A14" s="12" t="inlineStr">
         <is>
           <t>Liner TV AMI</t>
         </is>
       </c>
-      <c r="B14" s="12" t="inlineStr">
+      <c r="B14" s="13" t="inlineStr">
         <is>
           <t>{o_t_8}</t>
         </is>
       </c>
-      <c r="C14" s="12" t="inlineStr">
+      <c r="C14" s="13" t="inlineStr">
         <is>
           <t>{o_t_12}</t>
         </is>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="11" t="inlineStr">
+      <c r="A15" s="12" t="inlineStr">
         <is>
           <t>Meta AMI</t>
         </is>
       </c>
-      <c r="B15" s="12" t="inlineStr">
+      <c r="B15" s="13" t="inlineStr">
         <is>
           <t>{o_t_9}</t>
         </is>
       </c>
-      <c r="C15" s="12" t="inlineStr">
+      <c r="C15" s="13" t="inlineStr">
         <is>
           <t>{o_t_13}</t>
         </is>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="13" t="inlineStr">
+      <c r="A16" s="14" t="inlineStr">
         <is>
           <t>total</t>
         </is>
       </c>
-      <c r="B16" s="14" t="inlineStr">
+      <c r="B16" s="15" t="inlineStr">
         <is>
           <t>{o_t_10}</t>
         </is>
       </c>
-      <c r="C16" s="14" t="inlineStr">
+      <c r="C16" s="15" t="inlineStr">
         <is>
           <t>{o_t_14}</t>
         </is>
       </c>
     </row>
     <row r="17" ht="34" customHeight="1">
-      <c r="A17" s="15" t="inlineStr">
+      <c r="A17" s="16" t="inlineStr">
         <is>
           <t>total duplicated Net Campaign Reach</t>
         </is>
       </c>
-      <c r="B17" s="16" t="inlineStr">
+      <c r="B17" s="17" t="inlineStr">
         <is>
           <t>33, 714, 428</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="17" t="n"/>
-      <c r="B18" s="17" t="n"/>
+      <c r="A18" s="18" t="n"/>
+      <c r="B18" s="18" t="n"/>
     </row>
     <row r="19">
       <c r="H19" t="inlineStr">

</xml_diff>

<commit_message>
update on the template and tokens
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -19,7 +19,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -75,11 +75,19 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <color theme="0"/>
+      <sz val="14"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -106,13 +114,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2"/>
+        <fgColor theme="0" tint="-0.1499984740745262"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -129,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -145,17 +147,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -690,7 +689,7 @@
         <v>33714428</v>
       </c>
       <c r="G5" s="7" t="n">
-        <v>1203</v>
+        <v>61.34</v>
       </c>
     </row>
     <row r="6"/>
@@ -706,7 +705,7 @@
     </row>
     <row r="10"/>
     <row r="11"/>
-    <row r="12">
+    <row r="12" ht="19" customHeight="1">
       <c r="A12" s="10" t="n"/>
       <c r="B12" s="10" t="inlineStr">
         <is>
@@ -718,7 +717,11 @@
           <t>Unique Reach</t>
         </is>
       </c>
-      <c r="E12" s="11" t="n"/>
+      <c r="E12" s="11" t="inlineStr">
+        <is>
+          <t>Example Narrative:</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="12" t="inlineStr">
@@ -726,15 +729,11 @@
           <t>You Tube AMI</t>
         </is>
       </c>
-      <c r="B13" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_7}</t>
-        </is>
-      </c>
-      <c r="C13" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_11}</t>
-        </is>
+      <c r="B13" s="7" t="n">
+        <v>4433450</v>
+      </c>
+      <c r="C13" s="7" t="n">
+        <v>9604214</v>
       </c>
     </row>
     <row r="14">
@@ -743,14 +742,15 @@
           <t>Liner TV AMI</t>
         </is>
       </c>
-      <c r="B14" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_8}</t>
-        </is>
-      </c>
-      <c r="C14" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_12}</t>
+      <c r="B14" s="7" t="n">
+        <v>9724094</v>
+      </c>
+      <c r="C14" s="7" t="n">
+        <v>8514602</v>
+      </c>
+      <c r="E14" s="13" t="inlineStr">
+        <is>
+          <t>sample narrative for the report</t>
         </is>
       </c>
     </row>
@@ -760,15 +760,11 @@
           <t>Meta AMI</t>
         </is>
       </c>
-      <c r="B15" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_9}</t>
-        </is>
-      </c>
-      <c r="C15" s="13" t="inlineStr">
-        <is>
-          <t>{o_t_13}</t>
-        </is>
+      <c r="B15" s="7" t="n">
+        <v>6974566</v>
+      </c>
+      <c r="C15" s="7" t="n">
+        <v>1113865</v>
       </c>
     </row>
     <row r="16">
@@ -777,32 +773,29 @@
           <t>total</t>
         </is>
       </c>
-      <c r="B16" s="15" t="inlineStr">
-        <is>
-          <t>{o_t_10}</t>
-        </is>
-      </c>
-      <c r="C16" s="15" t="inlineStr">
-        <is>
-          <t>{o_t_14}</t>
-        </is>
-      </c>
+      <c r="B16" s="15" t="n">
+        <v>7287140</v>
+      </c>
+      <c r="C16" s="15" t="n">
+        <v>6927695</v>
+      </c>
+      <c r="E16" s="13" t="n"/>
     </row>
     <row r="17" ht="34" customHeight="1">
-      <c r="A17" s="16" t="inlineStr">
+      <c r="A17" s="13" t="inlineStr">
         <is>
           <t>total duplicated Net Campaign Reach</t>
         </is>
       </c>
-      <c r="B17" s="17" t="inlineStr">
+      <c r="B17" s="16" t="inlineStr">
         <is>
           <t>33, 714, 428</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="18" t="n"/>
-      <c r="B18" s="18" t="n"/>
+      <c r="A18" s="17" t="n"/>
+      <c r="B18" s="17" t="n"/>
     </row>
     <row r="19">
       <c r="H19" t="inlineStr">

</xml_diff>

<commit_message>
option to pass template as system args
</commit_message>
<xml_diff>
--- a/source/report_output/output.xlsx
+++ b/source/report_output/output.xlsx
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B13" s="7" t="n">
-        <v>4433450</v>
+        <v>5912805</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>9604214</v>
+        <v>159110</v>
       </c>
     </row>
     <row r="14">
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="B14" s="7" t="n">
-        <v>9724094</v>
+        <v>1807236</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>8514602</v>
+        <v>9642307</v>
       </c>
       <c r="E14" s="13" t="inlineStr">
         <is>
@@ -761,10 +761,10 @@
         </is>
       </c>
       <c r="B15" s="7" t="n">
-        <v>6974566</v>
+        <v>7449809</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>1113865</v>
+        <v>2294202</v>
       </c>
     </row>
     <row r="16">
@@ -774,10 +774,10 @@
         </is>
       </c>
       <c r="B16" s="15" t="n">
-        <v>7287140</v>
+        <v>9206617</v>
       </c>
       <c r="C16" s="15" t="n">
-        <v>6927695</v>
+        <v>7057512</v>
       </c>
       <c r="E16" s="13" t="n"/>
     </row>

</xml_diff>